<commit_message>
Si4 Mapping upgrade, custom field variables support
</commit_message>
<xml_diff>
--- a/docs/si4_model.xlsx
+++ b/docs/si4_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1400" windowWidth="22240" windowHeight="16540" tabRatio="796"/>
+    <workbookView xWindow="640" yWindow="1400" windowWidth="25180" windowHeight="16540" tabRatio="796" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="si4" sheetId="5" r:id="rId1"/>
@@ -2243,8 +2243,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1693">
+  <cellStyleXfs count="1697">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3963,7 +3967,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1693">
+  <cellStyles count="1697">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4810,6 +4814,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1688" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1690" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5656,6 +5662,8 @@
     <cellStyle name="Hyperlink" xfId="1687" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1689" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5955,7 +5963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
@@ -10511,15 +10519,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="163.6640625" customWidth="1"/>
+    <col min="2" max="2" width="89.5" customWidth="1"/>
     <col min="3" max="3" width="61" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" customWidth="1"/>
   </cols>
@@ -11166,8 +11174,8 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>